<commit_message>
reorganized the file structure
</commit_message>
<xml_diff>
--- a/進捗管理表.xlsx
+++ b/進捗管理表.xlsx
@@ -67,7 +67,46 @@
     <t>こさし</t>
   </si>
   <si>
-    <t>アイボリー背景色のセル値は列読み取りの基準なので変更しないでください。</t>
+    <t>曜日に
+「開」と記入することで土日、
+「休」「祝」と記入することで平日
+の扱いを上書きできます。</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">アイボリー背景色のセル値は列読み取り基準なので変更不可です。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FFFF00FF"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>タスクの増減や担当者の変更時はシートをコピー</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">してベースライン(計画)を更新してください。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FFFF00FF"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>編集はGoogleドライブ上でのみ</t>
+    </r>
   </si>
   <si>
     <t>リーダー</t>
@@ -80,9 +119,6 @@
   </si>
   <si>
     <t>ファシリテーター</t>
-  </si>
-  <si>
-    <t>タスクの増減や担当者の変更時はシートをコピーしてベースライン(計画)を更新してください。</t>
   </si>
   <si>
     <t>担当者の列は一部(K列からN列)非表示にしてあります。↑</t>
@@ -593,7 +629,7 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -603,6 +639,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -641,9 +680,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf borderId="9" fillId="3" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -1036,352 +1072,282 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
+      <c r="P2" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="AE2" s="4"/>
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+        <v>17</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="4"/>
-      <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="J4" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
+      <c r="O4" s="11"/>
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
       <c r="AG4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="J5" s="10"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
     </row>
     <row r="6">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="14"/>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="14"/>
-      <c r="AB6" s="14"/>
-      <c r="AC6" s="14"/>
-      <c r="AD6" s="14"/>
-      <c r="AE6" s="14"/>
-      <c r="AF6" s="14"/>
-      <c r="AG6" s="14"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="15"/>
+      <c r="AE6" s="15"/>
+      <c r="AF6" s="15"/>
+      <c r="AG6" s="15"/>
     </row>
     <row r="7">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="15" t="s">
+      <c r="N7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="17">
+      <c r="O7" s="18">
         <v>46035.0</v>
       </c>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
-      <c r="AB7" s="18"/>
-      <c r="AC7" s="18"/>
-      <c r="AD7" s="18"/>
-      <c r="AE7" s="18"/>
-      <c r="AF7" s="18"/>
-      <c r="AG7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="19"/>
+      <c r="AE7" s="19"/>
+      <c r="AF7" s="19"/>
+      <c r="AG7" s="20"/>
     </row>
     <row r="8">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="21">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="22">
         <f t="shared" ref="O8:O9" si="2">O7</f>
         <v>46035</v>
       </c>
-      <c r="P8" s="21">
+      <c r="P8" s="22">
         <f t="shared" ref="P8:AG8" si="1">O8+1</f>
         <v>46036</v>
       </c>
-      <c r="Q8" s="21">
+      <c r="Q8" s="22">
         <f t="shared" si="1"/>
         <v>46037</v>
       </c>
-      <c r="R8" s="21">
+      <c r="R8" s="22">
         <f t="shared" si="1"/>
         <v>46038</v>
       </c>
-      <c r="S8" s="21">
+      <c r="S8" s="22">
         <f t="shared" si="1"/>
         <v>46039</v>
       </c>
-      <c r="T8" s="21">
+      <c r="T8" s="22">
         <f t="shared" si="1"/>
         <v>46040</v>
       </c>
-      <c r="U8" s="21">
+      <c r="U8" s="22">
         <f t="shared" si="1"/>
         <v>46041</v>
       </c>
-      <c r="V8" s="21">
+      <c r="V8" s="22">
         <f t="shared" si="1"/>
         <v>46042</v>
       </c>
-      <c r="W8" s="21">
+      <c r="W8" s="22">
         <f t="shared" si="1"/>
         <v>46043</v>
       </c>
-      <c r="X8" s="21">
+      <c r="X8" s="22">
         <f t="shared" si="1"/>
         <v>46044</v>
       </c>
-      <c r="Y8" s="21">
+      <c r="Y8" s="22">
         <f t="shared" si="1"/>
         <v>46045</v>
       </c>
-      <c r="Z8" s="21">
+      <c r="Z8" s="22">
         <f t="shared" si="1"/>
         <v>46046</v>
       </c>
-      <c r="AA8" s="21">
+      <c r="AA8" s="22">
         <f t="shared" si="1"/>
         <v>46047</v>
       </c>
-      <c r="AB8" s="21">
+      <c r="AB8" s="22">
         <f t="shared" si="1"/>
         <v>46048</v>
       </c>
-      <c r="AC8" s="21">
+      <c r="AC8" s="22">
         <f t="shared" si="1"/>
         <v>46049</v>
       </c>
-      <c r="AD8" s="21">
+      <c r="AD8" s="22">
         <f t="shared" si="1"/>
         <v>46050</v>
       </c>
-      <c r="AE8" s="21">
+      <c r="AE8" s="22">
         <f t="shared" si="1"/>
         <v>46051</v>
       </c>
-      <c r="AF8" s="21">
+      <c r="AF8" s="22">
         <f t="shared" si="1"/>
         <v>46052</v>
       </c>
-      <c r="AG8" s="21">
+      <c r="AG8" s="22">
         <f t="shared" si="1"/>
         <v>46053</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="23">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="24">
         <f t="shared" si="2"/>
         <v>46035</v>
       </c>
@@ -5158,7 +5124,9 @@
         <v>105</v>
       </c>
       <c r="B93" s="6"/>
-      <c r="C93" s="31"/>
+      <c r="C93" s="31">
+        <v>46048.625</v>
+      </c>
       <c r="D93" s="31"/>
       <c r="E93" s="31"/>
       <c r="F93" s="33"/>
@@ -12614,26 +12582,28 @@
       <c r="A1018" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
     <mergeCell ref="H7:H9"/>
     <mergeCell ref="I7:I9"/>
     <mergeCell ref="J7:J9"/>
     <mergeCell ref="K7:K9"/>
     <mergeCell ref="L7:L9"/>
     <mergeCell ref="M7:M9"/>
-    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="P2:AD5"/>
     <mergeCell ref="O7:AG7"/>
+    <mergeCell ref="A3:D5"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="N7:N9"/>
   </mergeCells>
   <conditionalFormatting sqref="O8:AG218">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>OR(WEEKDAY(O$9,2)&gt;5, O$9="祝")</formula>
+      <formula>AND(O$9&lt;&gt;"開", OR(WEEKDAY(O$8,2)&gt;5, O$9="休", O$9="祝"))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions/>
@@ -12662,30 +12632,30 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
     </row>
     <row r="3">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4">
       <c r="A4" s="25" t="s">
@@ -12727,7 +12697,7 @@
       <c r="C7" s="31">
         <v>46050.395833333336</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="21"/>
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
@@ -12737,7 +12707,7 @@
       <c r="C8" s="31">
         <v>46050.395833333336</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="23"/>
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">

</xml_diff>

<commit_message>
docs: fix the unit of datetime on xlsx.
</commit_message>
<xml_diff>
--- a/進捗管理表.xlsx
+++ b/進捗管理表.xlsx
@@ -99,7 +99,7 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t>してベースライン(計画)を更新してください。</t>
+      <t>してベースライン名(計画名)を更新してください。</t>
     </r>
   </si>
   <si>
@@ -1438,10 +1438,12 @@
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="29">
-        <v>46035.541666666664</v>
+        <f> $O$5 + 46800/86400</f>
+        <v>46035.54167</v>
       </c>
       <c r="D9" s="29">
-        <v>46035.555555555555</v>
+        <f>C9 + 20 / 1440</f>
+        <v>46035.55556</v>
       </c>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
@@ -1487,10 +1489,12 @@
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="29">
-        <v>46035.555555555555</v>
+        <f> $O$5 + 48000/86400</f>
+        <v>46035.55556</v>
       </c>
       <c r="D10" s="29">
-        <v>46035.59722222222</v>
+        <f>C10 + 60 / 1440</f>
+        <v>46035.59722</v>
       </c>
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
@@ -1536,10 +1540,12 @@
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="29">
-        <v>46035.59722222222</v>
+        <f> $O$5 + 51600/86400</f>
+        <v>46035.59722</v>
       </c>
       <c r="D11" s="29">
-        <v>46035.666666666664</v>
+        <f>C11 + 100 / 1440</f>
+        <v>46035.66667</v>
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
@@ -1622,10 +1628,12 @@
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="29">
-        <v>46035.666666666664</v>
+        <f> $O$5 + 57600/86400</f>
+        <v>46035.66667</v>
       </c>
       <c r="D13" s="29">
-        <v>46035.708333333336</v>
+        <f>C13 + 60 / 1440</f>
+        <v>46035.70833</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
@@ -1708,10 +1716,12 @@
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="29">
+        <f> $O$5 + 118800/86400</f>
         <v>46036.375</v>
       </c>
       <c r="D15" s="29">
-        <v>46036.479166666664</v>
+        <f>C15 + 150 / 1440</f>
+        <v>46036.47917</v>
       </c>
       <c r="E15" s="29"/>
       <c r="F15" s="31"/>
@@ -1757,10 +1767,12 @@
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="29">
-        <v>46036.479166666664</v>
+        <f> $O$5 + 127800/86400</f>
+        <v>46036.47917</v>
       </c>
       <c r="D16" s="29">
-        <v>46036.48263888889</v>
+        <f>C16 + 5 / 1440</f>
+        <v>46036.48264</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="31"/>
@@ -1800,9 +1812,11 @@
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="29">
-        <v>46036.48263888889</v>
+        <f> $O$5 + 128100/86400</f>
+        <v>46036.48264</v>
       </c>
       <c r="D17" s="29">
+        <f>C17 + 25 / 1440</f>
         <v>46036.5</v>
       </c>
       <c r="E17" s="29"/>
@@ -1886,10 +1900,12 @@
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="29">
-        <v>46037.541666666664</v>
+        <f> $O$5 + 219600/86400</f>
+        <v>46037.54167</v>
       </c>
       <c r="D19" s="29">
-        <v>46037.583333333336</v>
+        <f>C19 + 60 / 1440</f>
+        <v>46037.58333</v>
       </c>
       <c r="E19" s="29"/>
       <c r="F19" s="31"/>
@@ -1935,10 +1951,12 @@
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="29">
-        <v>46037.583333333336</v>
+        <f> $O$5 + 223200/86400</f>
+        <v>46037.58333</v>
       </c>
       <c r="D20" s="29">
-        <v>46037.604166666664</v>
+        <f>C20 + 30 / 1440</f>
+        <v>46037.60417</v>
       </c>
       <c r="E20" s="29"/>
       <c r="F20" s="31"/>
@@ -2058,9 +2076,11 @@
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="29">
-        <v>46037.604166666664</v>
+        <f> $O$5 + 225000/86400</f>
+        <v>46037.60417</v>
       </c>
       <c r="D23" s="29">
+        <f>C23 + 30 / 1440</f>
         <v>46037.625</v>
       </c>
       <c r="E23" s="29"/>
@@ -2107,10 +2127,12 @@
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="29">
+        <f> $O$5 + 226800/86400</f>
         <v>46037.625</v>
       </c>
       <c r="D24" s="29">
-        <v>46037.666666666664</v>
+        <f>C24 + 60 / 1440</f>
+        <v>46037.66667</v>
       </c>
       <c r="E24" s="31"/>
       <c r="F24" s="31"/>
@@ -2156,10 +2178,12 @@
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="29">
-        <v>46037.666666666664</v>
+        <f> $O$5 + 230400/86400</f>
+        <v>46037.66667</v>
       </c>
       <c r="D25" s="29">
-        <v>46037.697916666664</v>
+        <f>C25 + 45 / 1440</f>
+        <v>46037.69792</v>
       </c>
       <c r="E25" s="29"/>
       <c r="F25" s="31"/>
@@ -2205,10 +2229,12 @@
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="29">
-        <v>46037.697916666664</v>
+        <f t="shared" ref="C26:C27" si="4"> $O$5 + 233100/86400</f>
+        <v>46037.69792</v>
       </c>
       <c r="D26" s="29">
-        <v>46037.708333333336</v>
+        <f t="shared" ref="D26:D27" si="5">C26 + 15 / 1440</f>
+        <v>46037.70833</v>
       </c>
       <c r="E26" s="29"/>
       <c r="F26" s="31"/>
@@ -2250,10 +2276,12 @@
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="29">
-        <v>46037.697916666664</v>
+        <f t="shared" si="4"/>
+        <v>46037.69792</v>
       </c>
       <c r="D27" s="29">
-        <v>46037.708333333336</v>
+        <f t="shared" si="5"/>
+        <v>46037.70833</v>
       </c>
       <c r="E27" s="29"/>
       <c r="F27" s="31"/>
@@ -2332,10 +2360,12 @@
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="29">
+        <f> $O$5 + 291600/86400</f>
         <v>46038.375</v>
       </c>
       <c r="D29" s="29">
-        <v>46038.458333333336</v>
+        <f>C29 + 120 / 1440</f>
+        <v>46038.45833</v>
       </c>
       <c r="E29" s="29"/>
       <c r="F29" s="31"/>
@@ -2381,9 +2411,11 @@
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="29">
-        <v>46038.458333333336</v>
+        <f> $O$5 + 298800/86400</f>
+        <v>46038.45833</v>
       </c>
       <c r="D30" s="29">
+        <f>C30 + 60 / 1440</f>
         <v>46038.5</v>
       </c>
       <c r="E30" s="29"/>
@@ -2430,10 +2462,12 @@
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="29">
-        <v>46038.541666666664</v>
+        <f> $O$5 + 306000/86400</f>
+        <v>46038.54167</v>
       </c>
       <c r="D31" s="29">
-        <v>46038.54861111111</v>
+        <f t="shared" ref="D31:D32" si="6">C31 + 10 / 1440</f>
+        <v>46038.54861</v>
       </c>
       <c r="E31" s="31"/>
       <c r="F31" s="31"/>
@@ -2475,10 +2509,12 @@
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="29">
-        <v>46038.54861111111</v>
+        <f> $O$5 + 306600/86400</f>
+        <v>46038.54861</v>
       </c>
       <c r="D32" s="29">
-        <v>46038.555555555555</v>
+        <f t="shared" si="6"/>
+        <v>46038.55556</v>
       </c>
       <c r="E32" s="31"/>
       <c r="F32" s="31"/>
@@ -2520,10 +2556,12 @@
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="29">
-        <v>46038.541666666664</v>
+        <f> $O$5 + 306000/86400</f>
+        <v>46038.54167</v>
       </c>
       <c r="D33" s="29">
-        <v>46038.666666666664</v>
+        <f>C33 + 180 / 1440</f>
+        <v>46038.66667</v>
       </c>
       <c r="E33" s="31"/>
       <c r="F33" s="31"/>
@@ -2565,10 +2603,12 @@
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="29">
-        <v>46038.555555555555</v>
+        <f> $O$5 + 307200/86400</f>
+        <v>46038.55556</v>
       </c>
       <c r="D34" s="29">
-        <v>46038.666666666664</v>
+        <f>C34 + 160 / 1440</f>
+        <v>46038.66667</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
@@ -2609,7 +2649,7 @@
         <v>57</v>
       </c>
       <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
+      <c r="C35" s="33"/>
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
       <c r="F35" s="24"/>
@@ -2647,10 +2687,12 @@
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="29">
-        <v>46038.666666666664</v>
+        <f> $O$5 + 316800/86400</f>
+        <v>46038.66667</v>
       </c>
       <c r="D36" s="29">
-        <v>46038.708333333336</v>
+        <f>C36 + 60 / 1440</f>
+        <v>46038.70833</v>
       </c>
       <c r="E36" s="29"/>
       <c r="F36" s="31"/>
@@ -2696,10 +2738,12 @@
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="29">
+        <f> $O$5 + 550800/86400</f>
         <v>46041.375</v>
       </c>
       <c r="D37" s="29">
-        <v>46041.37847222222</v>
+        <f t="shared" ref="D37:D38" si="7">C37 + 5 / 1440</f>
+        <v>46041.37847</v>
       </c>
       <c r="E37" s="29"/>
       <c r="F37" s="31"/>
@@ -2745,10 +2789,12 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="29">
-        <v>46041.37847222222</v>
+        <f> $O$5 + 551100/86400</f>
+        <v>46041.37847</v>
       </c>
       <c r="D38" s="29">
-        <v>46041.381944444445</v>
+        <f t="shared" si="7"/>
+        <v>46041.38194</v>
       </c>
       <c r="E38" s="29"/>
       <c r="F38" s="31"/>
@@ -2794,10 +2840,12 @@
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="29">
-        <v>46041.381944444445</v>
+        <f t="shared" ref="C39:C42" si="8"> $O$5 + 551400/86400</f>
+        <v>46041.38194</v>
       </c>
       <c r="D39" s="29">
-        <v>46041.395833333336</v>
+        <f t="shared" ref="D39:D42" si="9">C39 + 20 / 1440</f>
+        <v>46041.39583</v>
       </c>
       <c r="E39" s="29"/>
       <c r="F39" s="31"/>
@@ -2837,10 +2885,12 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="29">
-        <v>46041.381944444445</v>
+        <f t="shared" si="8"/>
+        <v>46041.38194</v>
       </c>
       <c r="D40" s="29">
-        <v>46041.395833333336</v>
+        <f t="shared" si="9"/>
+        <v>46041.39583</v>
       </c>
       <c r="E40" s="29"/>
       <c r="F40" s="31"/>
@@ -2880,10 +2930,12 @@
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="29">
-        <v>46041.381944444445</v>
+        <f t="shared" si="8"/>
+        <v>46041.38194</v>
       </c>
       <c r="D41" s="29">
-        <v>46041.395833333336</v>
+        <f t="shared" si="9"/>
+        <v>46041.39583</v>
       </c>
       <c r="E41" s="29"/>
       <c r="F41" s="31"/>
@@ -2923,10 +2975,12 @@
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="29">
-        <v>46041.381944444445</v>
+        <f t="shared" si="8"/>
+        <v>46041.38194</v>
       </c>
       <c r="D42" s="29">
-        <v>46041.395833333336</v>
+        <f t="shared" si="9"/>
+        <v>46041.39583</v>
       </c>
       <c r="E42" s="29"/>
       <c r="F42" s="31"/>
@@ -2966,9 +3020,11 @@
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="29">
-        <v>46041.395833333336</v>
+        <f t="shared" ref="C43:C45" si="10"> $O$5 + 552600/86400</f>
+        <v>46041.39583</v>
       </c>
       <c r="D43" s="29">
+        <f t="shared" ref="D43:D45" si="11">C43 + 60 / 1440</f>
         <v>46041.4375</v>
       </c>
       <c r="E43" s="29"/>
@@ -3011,9 +3067,11 @@
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="29">
-        <v>46041.395833333336</v>
+        <f t="shared" si="10"/>
+        <v>46041.39583</v>
       </c>
       <c r="D44" s="29">
+        <f t="shared" si="11"/>
         <v>46041.4375</v>
       </c>
       <c r="E44" s="29"/>
@@ -3054,9 +3112,11 @@
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="29">
-        <v>46041.395833333336</v>
+        <f t="shared" si="10"/>
+        <v>46041.39583</v>
       </c>
       <c r="D45" s="29">
+        <f t="shared" si="11"/>
         <v>46041.4375</v>
       </c>
       <c r="E45" s="31"/>
@@ -3097,9 +3157,11 @@
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="29">
+        <f t="shared" ref="C46:C49" si="12"> $O$5 + 556200/86400</f>
         <v>46041.4375</v>
       </c>
       <c r="D46" s="29">
+        <f t="shared" ref="D46:D49" si="13">C46 + 1530 / 1440</f>
         <v>46042.5</v>
       </c>
       <c r="E46" s="29"/>
@@ -3140,9 +3202,11 @@
       </c>
       <c r="B47" s="11"/>
       <c r="C47" s="29">
+        <f t="shared" si="12"/>
         <v>46041.4375</v>
       </c>
       <c r="D47" s="29">
+        <f t="shared" si="13"/>
         <v>46042.5</v>
       </c>
       <c r="E47" s="29"/>
@@ -3183,9 +3247,11 @@
       </c>
       <c r="B48" s="11"/>
       <c r="C48" s="29">
+        <f t="shared" si="12"/>
         <v>46041.4375</v>
       </c>
       <c r="D48" s="29">
+        <f t="shared" si="13"/>
         <v>46042.5</v>
       </c>
       <c r="E48" s="31"/>
@@ -3226,9 +3292,11 @@
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="29">
+        <f t="shared" si="12"/>
         <v>46041.4375</v>
       </c>
       <c r="D49" s="29">
+        <f t="shared" si="13"/>
         <v>46042.5</v>
       </c>
       <c r="E49" s="29"/>
@@ -3269,10 +3337,12 @@
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="29">
-        <v>46042.541666666664</v>
+        <f> $O$5 + 651600/86400</f>
+        <v>46042.54167</v>
       </c>
       <c r="D50" s="29">
-        <v>46042.54513888889</v>
+        <f>C50 + 5 / 1440</f>
+        <v>46042.54514</v>
       </c>
       <c r="E50" s="29"/>
       <c r="F50" s="31"/>
@@ -3318,9 +3388,11 @@
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="29">
-        <v>46042.54513888889</v>
+        <f> $O$5 + 651900/86400</f>
+        <v>46042.54514</v>
       </c>
       <c r="D51" s="29">
+        <f>C51 + 115 / 1440</f>
         <v>46042.625</v>
       </c>
       <c r="E51" s="29"/>
@@ -3367,10 +3439,12 @@
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="29">
+        <f t="shared" ref="C52:C53" si="14"> $O$5 + 658800/86400</f>
         <v>46042.625</v>
       </c>
       <c r="D52" s="29">
-        <v>46042.62847222222</v>
+        <f t="shared" ref="D52:D53" si="15">C52 + 5 / 1440</f>
+        <v>46042.62847</v>
       </c>
       <c r="E52" s="29"/>
       <c r="F52" s="31"/>
@@ -3410,10 +3484,12 @@
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="29">
+        <f t="shared" si="14"/>
         <v>46042.625</v>
       </c>
       <c r="D53" s="29">
-        <v>46042.62847222222</v>
+        <f t="shared" si="15"/>
+        <v>46042.62847</v>
       </c>
       <c r="E53" s="29"/>
       <c r="F53" s="31"/>
@@ -3490,10 +3566,12 @@
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="29">
-        <v>46042.62847222222</v>
+        <f> $O$5 + 659100/86400</f>
+        <v>46042.62847</v>
       </c>
       <c r="D55" s="29">
-        <v>46042.645833333336</v>
+        <f>C55 + 25 / 1440</f>
+        <v>46042.64583</v>
       </c>
       <c r="E55" s="29"/>
       <c r="F55" s="31"/>
@@ -3535,10 +3613,12 @@
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="29">
-        <v>46042.645833333336</v>
+        <f t="shared" ref="C56:C58" si="16"> $O$5 + 660600/86400</f>
+        <v>46042.64583</v>
       </c>
       <c r="D56" s="29">
-        <v>46042.65277777778</v>
+        <f>C56 + 10 / 1440</f>
+        <v>46042.65278</v>
       </c>
       <c r="E56" s="29"/>
       <c r="F56" s="31"/>
@@ -3578,10 +3658,12 @@
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="29">
-        <v>46042.645833333336</v>
+        <f t="shared" si="16"/>
+        <v>46042.64583</v>
       </c>
       <c r="D57" s="29">
-        <v>46042.666666666664</v>
+        <f t="shared" ref="D57:D58" si="17">C57 + 30 / 1440</f>
+        <v>46042.66667</v>
       </c>
       <c r="E57" s="29"/>
       <c r="F57" s="31"/>
@@ -3621,10 +3703,12 @@
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="29">
-        <v>46042.645833333336</v>
+        <f t="shared" si="16"/>
+        <v>46042.64583</v>
       </c>
       <c r="D58" s="29">
-        <v>46042.666666666664</v>
+        <f t="shared" si="17"/>
+        <v>46042.66667</v>
       </c>
       <c r="E58" s="29"/>
       <c r="F58" s="31"/>
@@ -3666,10 +3750,12 @@
       </c>
       <c r="B59" s="8"/>
       <c r="C59" s="29">
-        <v>46042.666666666664</v>
+        <f t="shared" ref="C59:C60" si="18"> $O$5 + 662400/86400</f>
+        <v>46042.66667</v>
       </c>
       <c r="D59" s="29">
-        <v>46042.67361111111</v>
+        <f>C59 + 10 / 1440</f>
+        <v>46042.67361</v>
       </c>
       <c r="E59" s="29"/>
       <c r="F59" s="31"/>
@@ -3709,9 +3795,11 @@
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="29">
-        <v>46042.666666666664</v>
+        <f t="shared" si="18"/>
+        <v>46042.66667</v>
       </c>
       <c r="D60" s="29">
+        <f t="shared" ref="D60:D61" si="19">C60 + 30 / 1440</f>
         <v>46042.6875</v>
       </c>
       <c r="E60" s="29"/>
@@ -3752,10 +3840,12 @@
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="29">
+        <f> $O$5 + 664200/86400</f>
         <v>46042.6875</v>
       </c>
       <c r="D61" s="29">
-        <v>46042.708333333336</v>
+        <f t="shared" si="19"/>
+        <v>46042.70833</v>
       </c>
       <c r="E61" s="29"/>
       <c r="F61" s="31"/>
@@ -3797,10 +3887,12 @@
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="29">
+        <f t="shared" ref="C62:C63" si="20"> $O$5 + 723600/86400</f>
         <v>46043.375</v>
       </c>
       <c r="D62" s="29">
-        <v>46043.381944444445</v>
+        <f>C62 + 10 / 1440</f>
+        <v>46043.38194</v>
       </c>
       <c r="E62" s="29"/>
       <c r="F62" s="31"/>
@@ -3840,10 +3932,12 @@
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="29">
+        <f t="shared" si="20"/>
         <v>46043.375</v>
       </c>
       <c r="D63" s="29">
-        <v>46043.395833333336</v>
+        <f>C63 + 30 / 1440</f>
+        <v>46043.39583</v>
       </c>
       <c r="E63" s="29"/>
       <c r="F63" s="31"/>
@@ -3920,10 +4014,12 @@
       </c>
       <c r="B65" s="11"/>
       <c r="C65" s="29">
-        <v>46043.381944444445</v>
+        <f> $O$5 + 724200/86400</f>
+        <v>46043.38194</v>
       </c>
       <c r="D65" s="29">
-        <v>46043.458333333336</v>
+        <f>C65 + 110 / 1440</f>
+        <v>46043.45833</v>
       </c>
       <c r="E65" s="29"/>
       <c r="F65" s="29"/>
@@ -3965,10 +4061,12 @@
       </c>
       <c r="B66" s="11"/>
       <c r="C66" s="29">
-        <v>46043.395833333336</v>
+        <f> $O$5 + 725400/86400</f>
+        <v>46043.39583</v>
       </c>
       <c r="D66" s="29">
-        <v>46043.458333333336</v>
+        <f>C66 + 90 / 1440</f>
+        <v>46043.45833</v>
       </c>
       <c r="E66" s="29"/>
       <c r="F66" s="29"/>
@@ -4008,10 +4106,12 @@
       </c>
       <c r="B67" s="11"/>
       <c r="C67" s="29">
+        <f> $O$5 + 723600/86400</f>
         <v>46043.375</v>
       </c>
       <c r="D67" s="29">
-        <v>46043.458333333336</v>
+        <f>C67 + 120 / 1440</f>
+        <v>46043.45833</v>
       </c>
       <c r="E67" s="31"/>
       <c r="F67" s="31"/>
@@ -4051,9 +4151,11 @@
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="29">
-        <v>46043.458333333336</v>
+        <f> $O$5 + 730800/86400</f>
+        <v>46043.45833</v>
       </c>
       <c r="D68" s="29">
+        <f>C68 + 60 / 1440</f>
         <v>46043.5</v>
       </c>
       <c r="E68" s="29"/>
@@ -4100,10 +4202,12 @@
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="29">
-        <v>46043.541666666664</v>
+        <f> $O$5 + 738000/86400</f>
+        <v>46043.54167</v>
       </c>
       <c r="D69" s="29">
-        <v>46043.666666666664</v>
+        <f>C69 + 180 / 1440</f>
+        <v>46043.66667</v>
       </c>
       <c r="E69" s="29"/>
       <c r="F69" s="31"/>
@@ -4149,10 +4253,12 @@
       </c>
       <c r="B70" s="8"/>
       <c r="C70" s="29">
-        <v>46043.666666666664</v>
+        <f> $O$5 + 748800/86400</f>
+        <v>46043.66667</v>
       </c>
       <c r="D70" s="29">
-        <v>46043.67361111111</v>
+        <f>C70 + 10 / 1440</f>
+        <v>46043.67361</v>
       </c>
       <c r="E70" s="29"/>
       <c r="F70" s="31"/>
@@ -4198,10 +4304,12 @@
       </c>
       <c r="B71" s="8"/>
       <c r="C71" s="29">
-        <v>46043.67361111111</v>
+        <f t="shared" ref="C71:C72" si="21"> $O$5 + 749400/86400</f>
+        <v>46043.67361</v>
       </c>
       <c r="D71" s="29">
-        <v>46043.677083333336</v>
+        <f t="shared" ref="D71:D72" si="22">C71 + 5 / 1440</f>
+        <v>46043.67708</v>
       </c>
       <c r="E71" s="29"/>
       <c r="F71" s="31"/>
@@ -4241,10 +4349,12 @@
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="29">
-        <v>46043.67361111111</v>
+        <f t="shared" si="21"/>
+        <v>46043.67361</v>
       </c>
       <c r="D72" s="29">
-        <v>46043.677083333336</v>
+        <f t="shared" si="22"/>
+        <v>46043.67708</v>
       </c>
       <c r="E72" s="29"/>
       <c r="F72" s="31"/>
@@ -4321,10 +4431,12 @@
       </c>
       <c r="B74" s="8"/>
       <c r="C74" s="29">
-        <v>46043.677083333336</v>
+        <f> $O$5 + 749700/86400</f>
+        <v>46043.67708</v>
       </c>
       <c r="D74" s="29">
-        <v>46043.680555555555</v>
+        <f>C74 + 5 / 1440</f>
+        <v>46043.68056</v>
       </c>
       <c r="E74" s="29"/>
       <c r="F74" s="31"/>
@@ -4364,10 +4476,12 @@
       </c>
       <c r="B75" s="8"/>
       <c r="C75" s="29">
-        <v>46043.680555555555</v>
+        <f> $O$5 + 750000/86400</f>
+        <v>46043.68056</v>
       </c>
       <c r="D75" s="29">
-        <v>46043.708333333336</v>
+        <f>C75 + 40 / 1440</f>
+        <v>46043.70833</v>
       </c>
       <c r="E75" s="29"/>
       <c r="F75" s="31"/>
@@ -4413,10 +4527,12 @@
       </c>
       <c r="B76" s="8"/>
       <c r="C76" s="29">
+        <f> $O$5 + 810000/86400</f>
         <v>46044.375</v>
       </c>
       <c r="D76" s="29">
-        <v>46044.37847222222</v>
+        <f t="shared" ref="D76:D77" si="23">C76 + 5 / 1440</f>
+        <v>46044.37847</v>
       </c>
       <c r="E76" s="29"/>
       <c r="F76" s="31"/>
@@ -4456,10 +4572,12 @@
       </c>
       <c r="B77" s="8"/>
       <c r="C77" s="29">
-        <v>46044.37847222222</v>
+        <f> $O$5 + 810300/86400</f>
+        <v>46044.37847</v>
       </c>
       <c r="D77" s="29">
-        <v>46044.381944444445</v>
+        <f t="shared" si="23"/>
+        <v>46044.38194</v>
       </c>
       <c r="E77" s="29"/>
       <c r="F77" s="31"/>
@@ -4501,10 +4619,12 @@
       </c>
       <c r="B78" s="8"/>
       <c r="C78" s="29">
-        <v>46044.381944444445</v>
+        <f t="shared" ref="C78:C79" si="24"> $O$5 + 810600/86400</f>
+        <v>46044.38194</v>
       </c>
       <c r="D78" s="29">
-        <v>46044.458333333336</v>
+        <f t="shared" ref="D78:D79" si="25">C78 + 110 / 1440</f>
+        <v>46044.45833</v>
       </c>
       <c r="E78" s="29"/>
       <c r="F78" s="31"/>
@@ -4546,10 +4666,12 @@
       </c>
       <c r="B79" s="8"/>
       <c r="C79" s="29">
-        <v>46044.381944444445</v>
+        <f t="shared" si="24"/>
+        <v>46044.38194</v>
       </c>
       <c r="D79" s="29">
-        <v>46044.458333333336</v>
+        <f t="shared" si="25"/>
+        <v>46044.45833</v>
       </c>
       <c r="E79" s="29"/>
       <c r="F79" s="31"/>
@@ -4591,10 +4713,12 @@
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="29">
-        <v>46044.458333333336</v>
+        <f> $O$5 + 817200/86400</f>
+        <v>46044.45833</v>
       </c>
       <c r="D80" s="29">
-        <v>46044.708333333336</v>
+        <f>C80 + 360 / 1440</f>
+        <v>46044.70833</v>
       </c>
       <c r="E80" s="29"/>
       <c r="F80" s="31"/>
@@ -4640,10 +4764,12 @@
       </c>
       <c r="B81" s="8"/>
       <c r="C81" s="29">
+        <f> $O$5 + 896400/86400</f>
         <v>46045.375</v>
       </c>
       <c r="D81" s="29">
-        <v>46045.395833333336</v>
+        <f>C81 + 30 / 1440</f>
+        <v>46045.39583</v>
       </c>
       <c r="E81" s="29"/>
       <c r="F81" s="31"/>
@@ -4689,10 +4815,12 @@
       </c>
       <c r="B82" s="8"/>
       <c r="C82" s="29">
-        <v>46045.395833333336</v>
+        <f> $O$5 + 898200/86400</f>
+        <v>46045.39583</v>
       </c>
       <c r="D82" s="29">
-        <v>46045.583333333336</v>
+        <f>C82 + 270 / 1440</f>
+        <v>46045.58333</v>
       </c>
       <c r="E82" s="29"/>
       <c r="F82" s="31"/>
@@ -4738,10 +4866,12 @@
       </c>
       <c r="B83" s="8"/>
       <c r="C83" s="29">
-        <v>46045.583333333336</v>
+        <f> $O$5 + 914400/86400</f>
+        <v>46045.58333</v>
       </c>
       <c r="D83" s="29">
-        <v>46045.604166666664</v>
+        <f>C83 + 30 / 1440</f>
+        <v>46045.60417</v>
       </c>
       <c r="E83" s="29"/>
       <c r="F83" s="31"/>
@@ -4787,10 +4917,12 @@
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="29">
-        <v>46045.604166666664</v>
+        <f> $O$5 + 916200/86400</f>
+        <v>46045.60417</v>
       </c>
       <c r="D84" s="29">
-        <v>46045.60763888889</v>
+        <f>C84 + 5 / 1440</f>
+        <v>46045.60764</v>
       </c>
       <c r="E84" s="29"/>
       <c r="F84" s="31"/>
@@ -4829,7 +4961,7 @@
         <v>100</v>
       </c>
       <c r="B85" s="24"/>
-      <c r="C85" s="25"/>
+      <c r="C85" s="33"/>
       <c r="D85" s="24"/>
       <c r="E85" s="24"/>
       <c r="F85" s="24"/>
@@ -4867,10 +4999,12 @@
       </c>
       <c r="B86" s="8"/>
       <c r="C86" s="29">
-        <v>46045.60763888889</v>
+        <f t="shared" ref="C86:C88" si="26"> $O$5 + 916500/86400</f>
+        <v>46045.60764</v>
       </c>
       <c r="D86" s="29">
-        <v>46045.708333333336</v>
+        <f t="shared" ref="D86:D88" si="27">C86 + 145 / 1440</f>
+        <v>46045.70833</v>
       </c>
       <c r="E86" s="29"/>
       <c r="F86" s="31"/>
@@ -4912,10 +5046,12 @@
       </c>
       <c r="B87" s="8"/>
       <c r="C87" s="29">
-        <v>46045.60763888889</v>
+        <f t="shared" si="26"/>
+        <v>46045.60764</v>
       </c>
       <c r="D87" s="29">
-        <v>46045.708333333336</v>
+        <f t="shared" si="27"/>
+        <v>46045.70833</v>
       </c>
       <c r="E87" s="29"/>
       <c r="F87" s="31"/>
@@ -4955,10 +5091,12 @@
       </c>
       <c r="B88" s="8"/>
       <c r="C88" s="29">
-        <v>46045.60763888889</v>
+        <f t="shared" si="26"/>
+        <v>46045.60764</v>
       </c>
       <c r="D88" s="29">
-        <v>46045.708333333336</v>
+        <f t="shared" si="27"/>
+        <v>46045.70833</v>
       </c>
       <c r="E88" s="29"/>
       <c r="F88" s="31"/>
@@ -4998,9 +5136,11 @@
       </c>
       <c r="B89" s="8"/>
       <c r="C89" s="29">
+        <f> $O$5 + 1155600/86400</f>
         <v>46048.375</v>
       </c>
       <c r="D89" s="29">
+        <f>C89 + 360 / 1440</f>
         <v>46048.625</v>
       </c>
       <c r="E89" s="29"/>
@@ -5047,10 +5187,12 @@
       </c>
       <c r="B90" s="8"/>
       <c r="C90" s="29">
+        <f> $O$5 + 1177200/86400</f>
         <v>46048.625</v>
       </c>
       <c r="D90" s="29">
-        <v>46048.67013888889</v>
+        <f>C90 + 65 / 1440</f>
+        <v>46048.67014</v>
       </c>
       <c r="E90" s="29"/>
       <c r="F90" s="31"/>
@@ -5096,7 +5238,8 @@
       </c>
       <c r="B91" s="8"/>
       <c r="C91" s="29">
-        <v>46048.67013888889</v>
+        <f> $O$5 + 1181100/86400</f>
+        <v>46048.67014</v>
       </c>
       <c r="D91" s="29"/>
       <c r="E91" s="29"/>

</xml_diff>